<commit_message>
Added StatusControl, added error handling, shrinked EntryPoint designer code
</commit_message>
<xml_diff>
--- a/Sparta/Sparta.xlsx
+++ b/Sparta/Sparta.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="5595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21375" windowHeight="5655"/>
   </bookViews>
   <sheets>
-    <sheet name="EntryPoint" sheetId="2" r:id="rId1"/>
+    <sheet name="EntryPoint" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,27 +23,14 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -67,10 +54,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,50 +336,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:M4"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>